<commit_message>
This my Automation Project
</commit_message>
<xml_diff>
--- a/DemoWebShop/src/test/resources/testData/testData.xlsx
+++ b/DemoWebShop/src/test/resources/testData/testData.xlsx
@@ -1,13 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D99D7E3D-0CBC-4981-A604-4A66B25B14BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="39">
   <si>
     <t>no</t>
   </si>
@@ -121,12 +123,27 @@
   </si>
   <si>
     <t>vikas#123</t>
+  </si>
+  <si>
+    <t>TC_Register_003</t>
+  </si>
+  <si>
+    <t>Anusha</t>
+  </si>
+  <si>
+    <t>MK</t>
+  </si>
+  <si>
+    <t>anumk@gmail.com</t>
+  </si>
+  <si>
+    <t>anumk#9669</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -448,23 +465,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -484,10 +501,13 @@
         <v>33</v>
       </c>
       <c r="G1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -507,10 +527,13 @@
         <v>20</v>
       </c>
       <c r="G2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -530,10 +553,13 @@
         <v>21</v>
       </c>
       <c r="G3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -553,10 +579,13 @@
         <v>22</v>
       </c>
       <c r="G4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -576,10 +605,13 @@
         <v>23</v>
       </c>
       <c r="G5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -599,10 +631,13 @@
         <v>24</v>
       </c>
       <c r="G6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -622,10 +657,13 @@
         <v>25</v>
       </c>
       <c r="G7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -645,19 +683,22 @@
         <v>33</v>
       </c>
       <c r="G8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8" t="s">
         <v>1</v>
       </c>
-      <c r="H8" t="s">
-        <v>30</v>
-      </c>
       <c r="I8" t="s">
         <v>30</v>
       </c>
       <c r="J8" t="s">
+        <v>30</v>
+      </c>
+      <c r="K8" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -677,7 +718,7 @@
         <v>20</v>
       </c>
       <c r="G9" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="H9" t="s">
         <v>30</v>
@@ -686,10 +727,13 @@
         <v>30</v>
       </c>
       <c r="J9" t="s">
+        <v>30</v>
+      </c>
+      <c r="K9" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -709,7 +753,7 @@
         <v>21</v>
       </c>
       <c r="G10" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="H10" t="s">
         <v>30</v>
@@ -718,10 +762,13 @@
         <v>30</v>
       </c>
       <c r="J10" t="s">
+        <v>30</v>
+      </c>
+      <c r="K10" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -741,7 +788,7 @@
         <v>22</v>
       </c>
       <c r="G11" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="H11" t="s">
         <v>30</v>
@@ -750,10 +797,13 @@
         <v>30</v>
       </c>
       <c r="J11" t="s">
+        <v>30</v>
+      </c>
+      <c r="K11" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -773,7 +823,7 @@
         <v>23</v>
       </c>
       <c r="G12" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="H12" t="s">
         <v>30</v>
@@ -782,10 +832,13 @@
         <v>30</v>
       </c>
       <c r="J12" t="s">
+        <v>30</v>
+      </c>
+      <c r="K12" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -805,7 +858,7 @@
         <v>24</v>
       </c>
       <c r="G13" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="H13" t="s">
         <v>30</v>
@@ -814,10 +867,13 @@
         <v>30</v>
       </c>
       <c r="J13" t="s">
+        <v>30</v>
+      </c>
+      <c r="K13" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>29</v>
       </c>
@@ -837,7 +893,7 @@
         <v>25</v>
       </c>
       <c r="G14" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="H14" t="s">
         <v>30</v>
@@ -846,10 +902,13 @@
         <v>30</v>
       </c>
       <c r="J14" t="s">
+        <v>30</v>
+      </c>
+      <c r="K14" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -869,19 +928,22 @@
         <v>33</v>
       </c>
       <c r="G15" t="s">
+        <v>33</v>
+      </c>
+      <c r="H15" t="s">
         <v>1</v>
       </c>
-      <c r="H15" t="s">
-        <v>30</v>
-      </c>
       <c r="I15" t="s">
         <v>30</v>
       </c>
       <c r="J15" t="s">
+        <v>30</v>
+      </c>
+      <c r="K15" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>29</v>
       </c>
@@ -901,7 +963,7 @@
         <v>20</v>
       </c>
       <c r="G16" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="H16" t="s">
         <v>30</v>
@@ -910,27 +972,196 @@
         <v>30</v>
       </c>
       <c r="J16" t="s">
+        <v>30</v>
+      </c>
+      <c r="K16" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" t="s">
+        <v>36</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F17" t="s">
+        <v>38</v>
+      </c>
+      <c r="G17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F18" t="s">
+        <v>24</v>
+      </c>
+      <c r="G18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F19" t="s">
+        <v>25</v>
+      </c>
+      <c r="G19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F20" t="s">
+        <v>33</v>
+      </c>
+      <c r="G20" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F21" t="s">
+        <v>20</v>
+      </c>
+      <c r="G21" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E1" r:id="rId1"/>
-    <hyperlink ref="E2" r:id="rId2"/>
-    <hyperlink ref="E3" r:id="rId3"/>
-    <hyperlink ref="E4" r:id="rId4"/>
-    <hyperlink ref="E5" r:id="rId5"/>
-    <hyperlink ref="E6" r:id="rId6"/>
-    <hyperlink ref="E7" r:id="rId7"/>
-    <hyperlink ref="E9" r:id="rId8"/>
-    <hyperlink ref="E10" r:id="rId9"/>
-    <hyperlink ref="E11" r:id="rId10"/>
-    <hyperlink ref="E12" r:id="rId11"/>
-    <hyperlink ref="E13" r:id="rId12"/>
-    <hyperlink ref="E14" r:id="rId13"/>
-    <hyperlink ref="E16" r:id="rId14"/>
-    <hyperlink ref="E8" r:id="rId15"/>
-    <hyperlink ref="E15" r:id="rId16"/>
+    <hyperlink ref="E1" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="E3" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="E4" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="E5" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="E6" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="E7" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="E9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="E10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="E11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="E12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="E13" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="E14" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="E16" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="E8" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="E15" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="E17" r:id="rId17" xr:uid="{4B292A3D-8B24-4850-92F9-216323A14FEA}"/>
+    <hyperlink ref="E18" r:id="rId18" xr:uid="{A15AE5D0-AC1A-491D-9B9B-32DBE8F77368}"/>
+    <hyperlink ref="E19" r:id="rId19" xr:uid="{D014D531-A8E0-4186-A495-BD2C1549B780}"/>
+    <hyperlink ref="E21" r:id="rId20" xr:uid="{3A629C22-C267-4B7A-9FF8-5F88FBCEF80F}"/>
+    <hyperlink ref="E20" r:id="rId21" xr:uid="{23C0A976-CB51-4E4B-B609-33BBAAE815CB}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89F27723-081A-444D-96F7-5027764FD020}">
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="17.77734375" customWidth="1"/>
+    <col min="6" max="6" width="14.88671875" customWidth="1"/>
+    <col min="7" max="7" width="13.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E1" r:id="rId1" xr:uid="{61937BF2-1F13-4109-9CCD-5441AE329494}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>